<commit_message>
Undo modification for test
Signed-off-by: rh <githubrh@pm.me>
</commit_message>
<xml_diff>
--- a/LWA-352 Antenna Status & System Configuration.xlsx
+++ b/LWA-352 Antenna Status & System Configuration.xlsx
@@ -638,29 +638,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="3" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="4" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="4" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="4" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="4" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="5" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="5" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="26" min="25" style="6" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="37.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="3" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="4" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="4" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="4" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="4" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="5" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="5" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="26" min="25" style="6" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="1" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3878,7 +3878,7 @@
         <v>13</v>
       </c>
       <c r="K4" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L4" s="4" t="n">
         <v>11</v>

</xml_diff>

<commit_message>
pretest change for demo
Signed-off-by: rh <githubrh@pm.me>
</commit_message>
<xml_diff>
--- a/LWA-352 Antenna Status & System Configuration.xlsx
+++ b/LWA-352 Antenna Status & System Configuration.xlsx
@@ -638,29 +638,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="3" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="4" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="4" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="4" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="4" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="5" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="5" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="26" min="25" style="6" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.5"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="3" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="4" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="4" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="4" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="4" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="5" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="5" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="26" min="25" style="6" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="1" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3878,7 +3878,7 @@
         <v>13</v>
       </c>
       <c r="K4" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L4" s="4" t="n">
         <v>11</v>

</xml_diff>

<commit_message>
Fix location errors. All ants are on 1 snap
Signed-off-by: rh <githubrh@pm.me>
</commit_message>
<xml_diff>
--- a/LWA-352 Antenna Status & System Configuration.xlsx
+++ b/LWA-352 Antenna Status & System Configuration.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="108">
   <si>
     <t xml:space="preserve">dict_key</t>
   </si>
@@ -312,9 +312,6 @@
   </si>
   <si>
     <t xml:space="preserve">LWA-233</t>
-  </si>
-  <si>
-    <t xml:space="preserve">snap03.sas.pvt</t>
   </si>
   <si>
     <t xml:space="preserve">LWA-234</t>
@@ -631,35 +628,35 @@
   <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="E3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="E10" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+      <selection pane="bottomLeft" activeCell="N34" activeCellId="0" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="3" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="3" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="15.3877551020408"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="4" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="4" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="4" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="4" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="4" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="4" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="4" width="7.83163265306122"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="5" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="5" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="5" width="7.29081632653061"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="5" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="5" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="26" min="25" style="6" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="5" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="26" min="25" style="6" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="25.3775510204082"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -3875,13 +3872,13 @@
         <v>5</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K4" s="4" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="L4" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M4" s="0"/>
       <c r="N4" s="0" t="s">
@@ -3951,13 +3948,13 @@
         <v>5</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K5" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M5" s="0"/>
       <c r="N5" s="0" t="s">
@@ -4027,13 +4024,13 @@
         <v>5</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K6" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L6" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M6" s="0"/>
       <c r="N6" s="0" t="s">
@@ -4103,13 +4100,13 @@
         <v>5</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K7" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L7" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M7" s="0"/>
       <c r="N7" s="0" t="s">
@@ -4179,13 +4176,13 @@
         <v>5</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K8" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L8" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M8" s="0"/>
       <c r="N8" s="0" t="s">
@@ -4255,13 +4252,13 @@
         <v>5</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K9" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L9" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M9" s="0"/>
       <c r="N9" s="0" t="s">
@@ -4331,13 +4328,13 @@
         <v>5</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K10" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L10" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M10" s="0"/>
       <c r="N10" s="0" t="s">
@@ -4407,13 +4404,13 @@
         <v>6</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K11" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L11" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M11" s="0"/>
       <c r="N11" s="0" t="s">
@@ -4473,13 +4470,13 @@
         <v>3</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K12" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L12" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M12" s="0"/>
       <c r="N12" s="0" t="s">
@@ -4539,13 +4536,13 @@
         <v>4</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K13" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L13" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M13" s="0"/>
       <c r="N13" s="0" t="s">
@@ -4605,13 +4602,13 @@
         <v>3</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K14" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L14" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M14" s="0"/>
       <c r="N14" s="0" t="s">
@@ -4671,13 +4668,13 @@
         <v>4</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K15" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L15" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M15" s="0"/>
       <c r="N15" s="0" t="s">
@@ -4737,13 +4734,13 @@
         <v>4</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K16" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L16" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M16" s="0"/>
       <c r="N16" s="0" t="s">
@@ -4803,13 +4800,13 @@
         <v>88</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K17" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L17" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M17" s="0"/>
       <c r="N17" s="0" t="s">
@@ -4869,13 +4866,13 @@
         <v>4</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K18" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L18" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M18" s="0"/>
       <c r="N18" s="0" t="s">
@@ -4935,13 +4932,13 @@
         <v>4</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K19" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L19" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M19" s="0"/>
       <c r="N19" s="0" t="s">
@@ -5001,17 +4998,17 @@
         <v>4</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K20" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L20" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M20" s="0"/>
       <c r="N20" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O20" s="17" t="n">
         <v>1</v>
@@ -5043,7 +5040,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" s="21" t="n">
         <v>37.23984736</v>
@@ -5067,17 +5064,17 @@
         <v>88</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K21" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L21" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M21" s="0"/>
       <c r="N21" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O21" s="4" t="n">
         <v>1</v>
@@ -5109,7 +5106,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C22" s="15" t="n">
         <v>37.23982881</v>
@@ -5133,17 +5130,17 @@
         <v>4</v>
       </c>
       <c r="J22" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K22" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L22" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M22" s="0"/>
       <c r="N22" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O22" s="17" t="n">
         <v>1</v>
@@ -5175,7 +5172,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23" s="15" t="n">
         <v>37.2397921</v>
@@ -5199,17 +5196,17 @@
         <v>4</v>
       </c>
       <c r="J23" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K23" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L23" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M23" s="0"/>
       <c r="N23" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O23" s="17" t="n">
         <v>1</v>
@@ -5241,7 +5238,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C24" s="15" t="n">
         <v>37.23975704</v>
@@ -5265,17 +5262,17 @@
         <v>4</v>
       </c>
       <c r="J24" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K24" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L24" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M24" s="0"/>
       <c r="N24" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O24" s="17" t="n">
         <v>1</v>
@@ -5307,7 +5304,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C25" s="15" t="n">
         <v>37.2397385</v>
@@ -5331,17 +5328,17 @@
         <v>4</v>
       </c>
       <c r="J25" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K25" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L25" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M25" s="0"/>
       <c r="N25" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O25" s="17" t="n">
         <v>1</v>
@@ -5373,7 +5370,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" s="15" t="n">
         <v>37.23968976</v>
@@ -5397,17 +5394,17 @@
         <v>4</v>
       </c>
       <c r="J26" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K26" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L26" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M26" s="0"/>
       <c r="N26" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O26" s="17" t="n">
         <v>1</v>
@@ -5439,7 +5436,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C27" s="15" t="n">
         <v>37.23963868</v>
@@ -5463,17 +5460,17 @@
         <v>4</v>
       </c>
       <c r="J27" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K27" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L27" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M27" s="0"/>
       <c r="N27" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O27" s="17" t="n">
         <v>1</v>
@@ -5505,7 +5502,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C28" s="15" t="n">
         <v>37.23962331</v>
@@ -5529,17 +5526,17 @@
         <v>5</v>
       </c>
       <c r="J28" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K28" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L28" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M28" s="0"/>
       <c r="N28" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O28" s="17" t="n">
         <v>1</v>
@@ -5571,7 +5568,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C29" s="15" t="n">
         <v>37.23960332</v>
@@ -5595,17 +5592,17 @@
         <v>5</v>
       </c>
       <c r="J29" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K29" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L29" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M29" s="0"/>
       <c r="N29" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O29" s="17" t="n">
         <v>1</v>
@@ -5637,7 +5634,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C30" s="21" t="n">
         <v>37.23957759</v>
@@ -5661,17 +5658,17 @@
         <v>88</v>
       </c>
       <c r="J30" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K30" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L30" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M30" s="0"/>
       <c r="N30" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O30" s="4" t="n">
         <v>1</v>
@@ -5703,7 +5700,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C31" s="15" t="n">
         <v>37.23952126</v>
@@ -5727,17 +5724,17 @@
         <v>5</v>
       </c>
       <c r="J31" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K31" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L31" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M31" s="0"/>
       <c r="N31" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O31" s="17" t="n">
         <v>1</v>
@@ -5769,7 +5766,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C32" s="15" t="n">
         <v>37.23949967</v>
@@ -5793,17 +5790,17 @@
         <v>5</v>
       </c>
       <c r="J32" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K32" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L32" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M32" s="0"/>
       <c r="N32" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O32" s="17" t="n">
         <v>1</v>
@@ -5835,7 +5832,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C33" s="15" t="n">
         <v>37.23948833</v>
@@ -5859,17 +5856,17 @@
         <v>5</v>
       </c>
       <c r="J33" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K33" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L33" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M33" s="0"/>
       <c r="N33" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O33" s="17" t="n">
         <v>1</v>
@@ -5901,7 +5898,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C34" s="21" t="n">
         <v>37.2393934</v>
@@ -5925,17 +5922,17 @@
         <v>88</v>
       </c>
       <c r="J34" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K34" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L34" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M34" s="0"/>
       <c r="N34" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O34" s="4" t="n">
         <v>1</v>
@@ -5967,7 +5964,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C35" s="15" t="n">
         <v>37.23939119</v>
@@ -5991,17 +5988,17 @@
         <v>5</v>
       </c>
       <c r="J35" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K35" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L35" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M35" s="0"/>
       <c r="N35" s="0" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O35" s="17" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Fixed extra row which prevented parsing
Signed-off-by: rh <githubrh@pm.me>
</commit_message>
<xml_diff>
--- a/LWA-352 Antenna Status & System Configuration.xlsx
+++ b/LWA-352 Antenna Status & System Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://caltech.sharepoint.com/sites/ovro/projects/LWA Documents/WBS/WBS 02 - Physical Infrastructure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36C55B10-5E8B-4DED-AA95-A14F6E5D1F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{97CA1DF1-0ABF-47EF-9A9F-ECA1C53C1607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4119" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4091" uniqueCount="1139">
   <si>
     <t>influx tag</t>
   </si>
@@ -3388,12 +3388,6 @@
   </si>
   <si>
     <t>40 meter feed -- elevation given for 40m dish elevation axis</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
   <si>
     <t>LWA-366</t>
@@ -3680,7 +3674,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -4094,17 +4088,6 @@
     <border>
       <left/>
       <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -4212,7 +4195,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4393,15 +4376,15 @@
       <alignment horizontal="left" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -4412,55 +4395,55 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="32" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="31" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="38" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="15" fillId="8" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="37" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="38" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="37" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="15" fillId="8" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="15" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4476,7 +4459,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4485,21 +4468,21 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -4514,10 +4497,6 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -4528,10 +4507,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -4541,10 +4516,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -4563,10 +4534,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4584,16 +4551,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4620,29 +4579,17 @@
       <alignment horizontal="left" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -5012,8 +4959,8 @@
   <dimension ref="A1:AK370"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14:XFD14"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C357" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="A369" sqref="A369:XFD369"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
     </sheetView>
@@ -5070,37 +5017,37 @@
       <c r="D1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="95" t="s">
+      <c r="E1" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="95" t="s">
+      <c r="F1" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="99" t="s">
+      <c r="G1" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="102" t="s">
+      <c r="H1" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="102" t="s">
+      <c r="I1" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="105" t="s">
+      <c r="J1" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="105" t="s">
+      <c r="K1" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="109" t="s">
+      <c r="L1" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="109" t="s">
+      <c r="M1" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="105" t="s">
+      <c r="N1" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="105" t="s">
+      <c r="O1" s="102" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="90" t="s">
@@ -5135,7 +5082,7 @@
       <c r="AA1" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="121" t="s">
+      <c r="AB1" s="115" t="s">
         <v>25</v>
       </c>
       <c r="AC1" s="90" t="s">
@@ -5153,7 +5100,7 @@
       <c r="AG1" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="121" t="s">
+      <c r="AH1" s="115" t="s">
         <v>31</v>
       </c>
     </row>
@@ -5268,107 +5215,107 @@
       <c r="C3" s="92" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="94" t="s">
+      <c r="D3" s="93" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="96">
+      <c r="E3" s="95">
         <v>37.240452040000001</v>
       </c>
-      <c r="F3" s="98">
+      <c r="F3" s="96">
         <v>-118.2809073</v>
       </c>
-      <c r="G3" s="100">
+      <c r="G3" s="98">
         <v>1182.97</v>
       </c>
-      <c r="H3" s="103">
+      <c r="H3" s="100">
         <v>67.38</v>
       </c>
-      <c r="I3" s="104">
+      <c r="I3" s="101">
         <v>74.89</v>
       </c>
-      <c r="J3" s="106" t="s">
-        <v>69</v>
-      </c>
-      <c r="K3" s="108" t="s">
-        <v>69</v>
-      </c>
-      <c r="L3" s="110" t="s">
+      <c r="J3" s="103" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="104" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="M3" s="110" t="s">
+      <c r="M3" s="106" t="s">
         <v>71</v>
       </c>
-      <c r="N3" s="106" t="s">
+      <c r="N3" s="103" t="s">
         <v>72</v>
       </c>
-      <c r="O3" s="108" t="s">
+      <c r="O3" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="P3" s="114">
+      <c r="P3" s="109">
         <v>15</v>
       </c>
-      <c r="Q3" s="116">
+      <c r="Q3" s="110">
         <v>40</v>
       </c>
-      <c r="R3" s="116">
+      <c r="R3" s="110">
         <f>P3</f>
         <v>15</v>
       </c>
-      <c r="S3" s="116">
+      <c r="S3" s="110">
         <v>3</v>
       </c>
-      <c r="T3" s="117">
+      <c r="T3" s="111">
         <f>100 * $R3 + S3</f>
         <v>1503</v>
       </c>
-      <c r="U3" s="118">
+      <c r="U3" s="112">
         <v>4</v>
       </c>
-      <c r="V3" s="117">
+      <c r="V3" s="111">
         <f>100 * $R3 + U3</f>
         <v>1504</v>
       </c>
-      <c r="W3" s="119">
+      <c r="W3" s="113">
         <f>_xlfn.XLOOKUP(Y3,'SNAP2 IDs'!C$3:C$15,'SNAP2 IDs'!B$3:B$15,"")</f>
         <v>10</v>
       </c>
-      <c r="X3" s="116">
+      <c r="X3" s="110">
         <f>_xlfn.XLOOKUP($W3, 'SNAP2 IDs'!$B$3:$B$15,'SNAP2 IDs'!D$3:D$15, "Lookup err")</f>
         <v>1</v>
       </c>
-      <c r="Y3" s="116">
+      <c r="Y3" s="110">
         <v>3</v>
       </c>
-      <c r="Z3" s="116" t="str">
+      <c r="Z3" s="110" t="str">
         <f>_xlfn.XLOOKUP($W3, 'SNAP2 IDs'!$B$3:$B$15,'SNAP2 IDs'!E$3:E$15, "Lookup err")</f>
         <v>02:00:a6:4e:e4:6f</v>
       </c>
-      <c r="AA3" s="120" t="str">
+      <c r="AA3" s="114" t="str">
         <f>_xlfn.XLOOKUP($W3, 'SNAP2 IDs'!$B$3:$B$15,'SNAP2 IDs'!F$3:F$15, "Lookup err")</f>
         <v>snap03.sas.pvt</v>
       </c>
-      <c r="AB3" s="119">
+      <c r="AB3" s="113">
         <v>0</v>
       </c>
-      <c r="AC3" s="116">
+      <c r="AC3" s="110">
         <v>0</v>
       </c>
-      <c r="AD3" s="120">
+      <c r="AD3" s="114">
         <v>1</v>
       </c>
-      <c r="AE3" s="119">
+      <c r="AE3" s="113">
         <f>_xlfn.BITXOR(AC3,2) + 32*AB3</f>
         <v>2</v>
       </c>
-      <c r="AF3" s="120">
+      <c r="AF3" s="114">
         <f>_xlfn.BITXOR(AD3,2) + 32*AB3</f>
         <v>3</v>
       </c>
-      <c r="AG3" s="122">
+      <c r="AG3" s="116">
         <f>32*(Y3-1) + (AE3/2)</f>
         <v>65</v>
       </c>
-      <c r="AH3" s="123" t="s">
+      <c r="AH3" s="117" t="s">
         <v>73</v>
       </c>
     </row>
@@ -5414,7 +5361,7 @@
       <c r="R4" s="41"/>
       <c r="S4" s="41"/>
       <c r="T4" s="54"/>
-      <c r="U4" s="128"/>
+      <c r="U4" s="121"/>
       <c r="V4" s="54"/>
       <c r="W4" s="41"/>
       <c r="X4" s="41"/>
@@ -10027,7 +9974,7 @@
       <c r="P46" s="41">
         <v>17</v>
       </c>
-      <c r="Q46" s="124">
+      <c r="Q46" s="118">
         <v>23</v>
       </c>
       <c r="R46" s="41">
@@ -10923,7 +10870,7 @@
       <c r="P54" s="41">
         <v>20</v>
       </c>
-      <c r="Q54" s="126">
+      <c r="Q54" s="120">
         <v>33</v>
       </c>
       <c r="R54" s="41">
@@ -35681,7 +35628,7 @@
       <c r="K281" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="L281" s="111">
+      <c r="L281" s="107">
         <v>483</v>
       </c>
       <c r="M281" s="63" t="s">
@@ -35787,7 +35734,7 @@
       <c r="K282" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="L282" s="112" t="s">
+      <c r="L282" s="108" t="s">
         <v>869</v>
       </c>
       <c r="M282" s="63" t="s">
@@ -36329,7 +36276,7 @@
       <c r="P287" s="41">
         <v>6</v>
       </c>
-      <c r="Q287" s="125">
+      <c r="Q287" s="119">
         <v>4098</v>
       </c>
       <c r="R287" s="41">
@@ -36755,7 +36702,7 @@
       <c r="P291" s="41">
         <v>6</v>
       </c>
-      <c r="Q291" s="125">
+      <c r="Q291" s="119">
         <v>4098</v>
       </c>
       <c r="R291" s="41">
@@ -37075,7 +37022,7 @@
       <c r="P294" s="41">
         <v>6</v>
       </c>
-      <c r="Q294" s="125">
+      <c r="Q294" s="119">
         <v>4098</v>
       </c>
       <c r="R294" s="41">
@@ -37181,7 +37128,7 @@
       <c r="P295" s="41">
         <v>6</v>
       </c>
-      <c r="Q295" s="125">
+      <c r="Q295" s="119">
         <v>4098</v>
       </c>
       <c r="R295" s="41">
@@ -37501,7 +37448,7 @@
       <c r="P298" s="41">
         <v>6</v>
       </c>
-      <c r="Q298" s="125">
+      <c r="Q298" s="119">
         <v>4098</v>
       </c>
       <c r="R298" s="41">
@@ -37607,7 +37554,7 @@
       <c r="P299" s="41">
         <v>6</v>
       </c>
-      <c r="Q299" s="125">
+      <c r="Q299" s="119">
         <v>4098</v>
       </c>
       <c r="R299" s="41">
@@ -37820,7 +37767,7 @@
       <c r="P301" s="41">
         <v>6</v>
       </c>
-      <c r="Q301" s="125">
+      <c r="Q301" s="119">
         <v>4098</v>
       </c>
       <c r="R301" s="41">
@@ -45012,187 +44959,96 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="369" spans="1:34" s="36" customFormat="1" ht="18" customHeight="1">
+    <row r="369" spans="1:34" ht="18.75" hidden="1" customHeight="1">
       <c r="A369" s="59"/>
-      <c r="B369" s="127" t="s">
+      <c r="B369" s="58" t="s">
         <v>1111</v>
       </c>
-      <c r="C369" s="93"/>
-      <c r="D369" s="93" t="s">
-        <v>1111</v>
-      </c>
-      <c r="E369" s="97" t="s">
+      <c r="C369" s="81"/>
+      <c r="D369" s="48" t="s">
+        <v>803</v>
+      </c>
+      <c r="E369" s="48">
+        <v>37.232092000000002</v>
+      </c>
+      <c r="F369" s="48">
+        <v>-118.29558400000001</v>
+      </c>
+      <c r="G369" s="49">
+        <v>1177.8</v>
+      </c>
+      <c r="H369" s="49">
+        <v>-1235.02</v>
+      </c>
+      <c r="I369" s="49">
+        <v>-852.93</v>
+      </c>
+      <c r="J369" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="K369" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="L369" s="63" t="s">
+        <v>455</v>
+      </c>
+      <c r="M369" s="63" t="s">
         <v>1112</v>
       </c>
-      <c r="F369" s="97" t="s">
-        <v>1112</v>
-      </c>
-      <c r="G369" s="101" t="s">
-        <v>1112</v>
-      </c>
-      <c r="H369" s="101" t="s">
-        <v>1112</v>
-      </c>
-      <c r="I369" s="101" t="s">
-        <v>1112</v>
-      </c>
-      <c r="J369" s="107" t="s">
-        <v>1112</v>
-      </c>
-      <c r="K369" s="107" t="s">
-        <v>1112</v>
-      </c>
-      <c r="L369" s="113" t="s">
-        <v>1111</v>
-      </c>
-      <c r="M369" s="113" t="s">
-        <v>1111</v>
-      </c>
-      <c r="N369" s="93" t="s">
-        <v>1112</v>
-      </c>
-      <c r="O369" s="93" t="s">
-        <v>1112</v>
-      </c>
-      <c r="P369" s="115" t="s">
-        <v>1111</v>
-      </c>
-      <c r="Q369" s="115" t="s">
-        <v>1112</v>
-      </c>
-      <c r="R369" s="115" t="s">
-        <v>1112</v>
-      </c>
-      <c r="S369" s="115" t="s">
-        <v>1111</v>
-      </c>
-      <c r="T369" s="115" t="s">
-        <v>1112</v>
-      </c>
-      <c r="U369" s="129" t="s">
-        <v>1111</v>
-      </c>
-      <c r="V369" s="115" t="s">
-        <v>1112</v>
-      </c>
-      <c r="W369" s="115" t="s">
-        <v>1111</v>
-      </c>
-      <c r="X369" s="115" t="s">
-        <v>1111</v>
-      </c>
-      <c r="Y369" s="115" t="s">
-        <v>1111</v>
-      </c>
-      <c r="Z369" s="115" t="s">
-        <v>1112</v>
-      </c>
-      <c r="AA369" s="115" t="s">
-        <v>1112</v>
-      </c>
-      <c r="AB369" s="115" t="s">
-        <v>1111</v>
-      </c>
-      <c r="AC369" s="115" t="s">
-        <v>1111</v>
-      </c>
-      <c r="AD369" s="115" t="s">
-        <v>1111</v>
-      </c>
-      <c r="AE369" s="115"/>
-      <c r="AF369" s="115"/>
-      <c r="AG369" s="115"/>
-      <c r="AH369" s="130"/>
-    </row>
-    <row r="370" spans="1:34" ht="18.75" hidden="1" customHeight="1">
-      <c r="A370" s="59"/>
-      <c r="B370" s="58" t="s">
+      <c r="N369" s="41"/>
+      <c r="O369" s="41"/>
+      <c r="P369" s="41"/>
+      <c r="Q369" s="41" t="str">
+        <f>_xlfn.XLOOKUP(P369,'ARX IDs'!B$3:B$47,'ARX IDs'!C$3:C$47,"")</f>
+        <v/>
+      </c>
+      <c r="R369" s="41"/>
+      <c r="S369" s="41"/>
+      <c r="T369" s="54">
+        <f>100 * $R369 + S369</f>
+        <v>0</v>
+      </c>
+      <c r="U369" s="86"/>
+      <c r="V369" s="54">
+        <f>100 * $R369 + U369</f>
+        <v>0</v>
+      </c>
+      <c r="W369" s="41" t="str">
+        <f>IF(ISBLANK(Y369), "", _xlfn.XLOOKUP(Y369,'SNAP2 IDs'!C$3:C$15,'SNAP2 IDs'!B$3:B$15,""))</f>
+        <v/>
+      </c>
+      <c r="X369" s="41"/>
+      <c r="Y369" s="41"/>
+      <c r="Z369" s="41"/>
+      <c r="AA369" s="41"/>
+      <c r="AB369" s="41"/>
+      <c r="AC369" s="41"/>
+      <c r="AD369" s="41"/>
+      <c r="AE369" s="41"/>
+      <c r="AF369" s="41"/>
+      <c r="AG369" s="41"/>
+      <c r="AH369" s="87" t="s">
         <v>1113</v>
       </c>
-      <c r="C370" s="81"/>
-      <c r="D370" s="48" t="s">
-        <v>803</v>
-      </c>
-      <c r="E370" s="48">
-        <v>37.232092000000002</v>
-      </c>
-      <c r="F370" s="48">
-        <v>-118.29558400000001</v>
-      </c>
-      <c r="G370" s="49">
-        <v>1177.8</v>
-      </c>
-      <c r="H370" s="49">
-        <v>-1235.02</v>
-      </c>
-      <c r="I370" s="49">
-        <v>-852.93</v>
-      </c>
-      <c r="J370" s="56" t="s">
-        <v>199</v>
-      </c>
-      <c r="K370" s="56" t="s">
-        <v>199</v>
-      </c>
-      <c r="L370" s="63" t="s">
-        <v>455</v>
-      </c>
-      <c r="M370" s="63" t="s">
-        <v>1114</v>
-      </c>
-      <c r="N370" s="41"/>
-      <c r="O370" s="41"/>
-      <c r="P370" s="41"/>
-      <c r="Q370" s="41" t="str">
-        <f>_xlfn.XLOOKUP(P370,'ARX IDs'!B$3:B$47,'ARX IDs'!C$3:C$47,"")</f>
-        <v/>
-      </c>
-      <c r="R370" s="41"/>
-      <c r="S370" s="41"/>
-      <c r="T370" s="54">
-        <f>100 * $R370 + S370</f>
-        <v>0</v>
-      </c>
-      <c r="U370" s="86"/>
-      <c r="V370" s="54">
-        <f>100 * $R370 + U370</f>
-        <v>0</v>
-      </c>
-      <c r="W370" s="41" t="str">
-        <f>IF(ISBLANK(Y370), "", _xlfn.XLOOKUP(Y370,'SNAP2 IDs'!C$3:C$15,'SNAP2 IDs'!B$3:B$15,""))</f>
-        <v/>
-      </c>
-      <c r="X370" s="41"/>
-      <c r="Y370" s="41"/>
-      <c r="Z370" s="41"/>
-      <c r="AA370" s="41"/>
-      <c r="AB370" s="41"/>
-      <c r="AC370" s="41"/>
-      <c r="AD370" s="41"/>
-      <c r="AE370" s="41"/>
-      <c r="AF370" s="41"/>
-      <c r="AG370" s="41"/>
-      <c r="AH370" s="87" t="s">
-        <v>1115</v>
-      </c>
-    </row>
+    </row>
+    <row r="370" spans="1:34" ht="15"/>
   </sheetData>
   <sheetProtection sort="0" autoFilter="0"/>
-  <autoFilter ref="A3:AH370" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A3:AH369" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="9">
       <filters>
         <filter val="YES"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:AH370">
-      <sortCondition ref="B3:B370"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:AH369">
+      <sortCondition ref="B3:B369"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:AH1048576">
-    <sortCondition ref="B1:B1048576"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:AH1048575">
+    <sortCondition ref="B1:B1048575"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A1:XFD3 U297:U370 U4:U155 A371:XFD1048576 B4:C370 AH236:XFD370 AI235:XFD235 U236:U295 U157:U234 AH4:XFD234">
+  <conditionalFormatting sqref="A1:XFD3 U4:U155 A370:XFD1048576 AI235:XFD235 U236:U295 U157:U234 AH4:XFD234 U297:U369 B4:C369 AH236:XFD369">
     <cfRule type="expression" dxfId="2" priority="44">
       <formula>CELL("protect",A1)=1</formula>
     </cfRule>
@@ -45231,25 +45087,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="67" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C1" s="73" t="s">
         <v>1116</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="D1" s="76" t="s">
         <v>1117</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="E1" s="69" t="s">
         <v>1118</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="F1" s="68" t="s">
         <v>1119</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="G1" s="68" t="s">
         <v>1120</v>
-      </c>
-      <c r="F1" s="68" t="s">
-        <v>1121</v>
-      </c>
-      <c r="G1" s="68" t="s">
-        <v>1122</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -52561,61 +52417,61 @@
       </c>
     </row>
     <row r="254" spans="1:7">
-      <c r="A254" s="66" t="str">
-        <f>'LWA config'!B369</f>
-        <v>yes</v>
-      </c>
-      <c r="B254" s="74" t="str">
-        <f>'LWA config'!E369</f>
-        <v>no</v>
-      </c>
-      <c r="C254" s="74" t="str">
-        <f>'LWA config'!F369</f>
-        <v>no</v>
-      </c>
-      <c r="D254" s="72" t="str">
-        <f>'LWA config'!G369</f>
-        <v>no</v>
+      <c r="A254" s="66" t="e">
+        <f>'LWA config'!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B254" s="74" t="e">
+        <f>'LWA config'!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C254" s="74" t="e">
+        <f>'LWA config'!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D254" s="72" t="e">
+        <f>'LWA config'!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="E254" s="70" t="s">
         <v>114</v>
       </c>
       <c r="F254" s="65" t="e">
-        <f>('LWA config'!P369-1)*16+'LWA config'!S369-1</f>
-        <v>#VALUE!</v>
+        <f>('LWA config'!#REF!-1)*16+'LWA config'!#REF!-1</f>
+        <v>#REF!</v>
       </c>
       <c r="G254" s="65" t="e">
-        <f>('LWA config'!Y369-1)*64+_xlfn.BITXOR('LWA config'!AC369,2)+32*'LWA config'!AB369</f>
-        <v>#VALUE!</v>
+        <f>('LWA config'!#REF!-1)*64+_xlfn.BITXOR('LWA config'!#REF!,2)+32*'LWA config'!#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="255" spans="1:7">
-      <c r="A255" s="66" t="str">
-        <f>'LWA config'!B369</f>
-        <v>yes</v>
-      </c>
-      <c r="B255" s="74" t="str">
-        <f>'LWA config'!E369</f>
-        <v>no</v>
-      </c>
-      <c r="C255" s="74" t="str">
-        <f>'LWA config'!F369</f>
-        <v>no</v>
-      </c>
-      <c r="D255" s="72" t="str">
-        <f>'LWA config'!G369</f>
-        <v>no</v>
+      <c r="A255" s="66" t="e">
+        <f>'LWA config'!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B255" s="74" t="e">
+        <f>'LWA config'!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C255" s="74" t="e">
+        <f>'LWA config'!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D255" s="72" t="e">
+        <f>'LWA config'!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="E255" s="70" t="s">
         <v>443</v>
       </c>
       <c r="F255" s="65" t="e">
-        <f>('LWA config'!P369-1)*16+'LWA config'!U369-1</f>
-        <v>#VALUE!</v>
+        <f>('LWA config'!#REF!-1)*16+'LWA config'!#REF!-1</f>
+        <v>#REF!</v>
       </c>
       <c r="G255" s="65" t="e">
-        <f>('LWA config'!Y369-1)*64+_xlfn.BITXOR('LWA config'!AD369,2)+32*'LWA config'!AB369</f>
-        <v>#VALUE!</v>
+        <f>('LWA config'!#REF!-1)*64+_xlfn.BITXOR('LWA config'!#REF!,2)+32*'LWA config'!#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="256" spans="1:7">
@@ -65730,7 +65586,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="F3" s="29" t="str">
         <f t="shared" ref="F3:F15" si="1">IF(ISBLANK(C3), "", CONCATENATE(IF(C3 &lt; 10, "snap0", "snap"),C3,".sas.pvt"))</f>
@@ -65770,7 +65626,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="F5" s="29" t="str">
         <f t="shared" si="1"/>
@@ -65790,7 +65646,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="F6" s="29" t="str">
         <f>IF(ISBLANK(C6), "", CONCATENATE(IF(C6 &lt; 10, "snap0", "snap"),C6,".sas.pvt"))</f>
@@ -65810,7 +65666,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="F7" s="29" t="str">
         <f t="shared" si="1"/>
@@ -65830,7 +65686,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="F8" s="29" t="str">
         <f t="shared" si="1"/>
@@ -65850,7 +65706,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="F9" s="29" t="str">
         <f t="shared" si="1"/>
@@ -65870,7 +65726,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="F10" s="29" t="str">
         <f t="shared" si="1"/>
@@ -65906,7 +65762,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="F12" s="29" t="str">
         <f t="shared" si="1"/>
@@ -65942,7 +65798,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="F14" s="29" t="str">
         <f t="shared" si="1"/>
@@ -65962,7 +65818,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="F15" s="40" t="str">
         <f t="shared" si="1"/>
@@ -66405,7 +66261,7 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="22" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="C2" s="22"/>
     </row>
@@ -66414,7 +66270,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="5" spans="2:4" s="26" customFormat="1" ht="35.25" customHeight="1">
@@ -66422,7 +66278,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="6" spans="2:4" s="26" customFormat="1" ht="35.25" customHeight="1">
@@ -66430,7 +66286,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="7" spans="2:4" s="26" customFormat="1">
@@ -66438,7 +66294,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="8" spans="2:4" s="26" customFormat="1" ht="53.25" customHeight="1">
@@ -66446,7 +66302,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="9" spans="2:4" s="26" customFormat="1" ht="66" customHeight="1">
@@ -66454,7 +66310,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="10" spans="2:4" s="26" customFormat="1" ht="29.1">
@@ -66462,7 +66318,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="11" spans="2:4" s="26" customFormat="1">
@@ -66702,6 +66558,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="70f2d024-d81a-45b9-9f62-d57c478f1068" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a2c70659-2d8e-48dd-af6d-da2141f5031a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_Flow_SignoffStatus xmlns="a2c70659-2d8e-48dd-af6d-da2141f5031a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100969A852156D25941A1952AB04D85E27D" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5eef67676188517ce8897ed475640d98">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a2c70659-2d8e-48dd-af6d-da2141f5031a" xmlns:ns3="56c45531-4dc0-4ecf-b1f6-b3e259fe0aa2" xmlns:ns4="70f2d024-d81a-45b9-9f62-d57c478f1068" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffaa8982e33fc8c9e56a16149ecac6ba" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="a2c70659-2d8e-48dd-af6d-da2141f5031a"/>
@@ -66967,35 +66844,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="70f2d024-d81a-45b9-9f62-d57c478f1068" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a2c70659-2d8e-48dd-af6d-da2141f5031a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_Flow_SignoffStatus xmlns="a2c70659-2d8e-48dd-af6d-da2141f5031a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED493C1A-537F-4BAE-8579-6F19325E5F1A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B935988-6FEA-4668-8153-6BCAA385B436}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B935988-6FEA-4668-8153-6BCAA385B436}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3F821CB-369E-4104-A49A-9E03773B151F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3F821CB-369E-4104-A49A-9E03773B151F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED493C1A-537F-4BAE-8579-6F19325E5F1A}"/>
 </file>
</xml_diff>